<commit_message>
modified:   binance1.py 	modified:   binance_ETHUSDT_data.csv 	modified:   binance_ETHUSDT_data.xlsx
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,52 +433,52 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1575158400000</v>
+        <v>1572566400000</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>151.43000000</t>
+          <t>182.19000000</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>152.49000000</t>
+          <t>184.50000000</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>145.79000000</t>
+          <t>177.02000000</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>150.73000000</t>
+          <t>182.85000000</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>344178.14088000</t>
+          <t>331519.76963000</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>1575244799999</v>
+        <v>1572652799999</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>51148792.08299820</t>
+          <t>60092727.13917590</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>125550</v>
+        <v>154534</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>172849.45417000</t>
+          <t>176366.39217000</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>25693814.94443980</t>
+          <t>31984647.88420370</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -492,52 +492,52 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1575244800000</v>
+        <v>1572652800000</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>150.72000000</t>
+          <t>182.86000000</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>151.42000000</t>
+          <t>186.00000000</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>146.71000000</t>
+          <t>181.53000000</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>148.65000000</t>
+          <t>182.91000000</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>233839.09730000</t>
+          <t>179864.39739000</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>1575331199999</v>
+        <v>1572739199999</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>34768563.47186470</t>
+          <t>32936676.70820530</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>107070</v>
+        <v>107048</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>114158.87515000</t>
+          <t>89462.03413000</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>16974888.53770170</t>
+          <t>16385817.10280250</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -551,52 +551,52 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1575331200000</v>
+        <v>1572739200000</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>148.66000000</t>
+          <t>182.90000000</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>149.93000000</t>
+          <t>184.70000000</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>145.77000000</t>
+          <t>178.95000000</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>147.17000000</t>
+          <t>181.54000000</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>196329.22503000</t>
+          <t>232621.52147000</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>1575417599999</v>
+        <v>1572825599999</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>29061161.10177570</t>
+          <t>42260620.37702860</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>87660</v>
+        <v>109861</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>100293.62450000</t>
+          <t>117372.86999000</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>14844721.32424090</t>
+          <t>21322878.29060180</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -610,52 +610,52 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1575417600000</v>
+        <v>1572825600000</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>147.19000000</t>
+          <t>181.53000000</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>151.98000000</t>
+          <t>188.64000000</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>143.15000000</t>
+          <t>180.36000000</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>145.38000000</t>
+          <t>185.71000000</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>434430.62379000</t>
+          <t>321175.29134000</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>1575503999999</v>
+        <v>1572911999999</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>63840615.24391760</t>
+          <t>59357371.31413380</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>149648</v>
+        <v>147624</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>211404.51257000</t>
+          <t>174839.08251000</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>31089708.18797030</t>
+          <t>32310789.00236290</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -669,52 +669,52 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1575504000000</v>
+        <v>1572912000000</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>145.45000000</t>
+          <t>185.71000000</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>149.02000000</t>
+          <t>192.51000000</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>143.64000000</t>
+          <t>182.22000000</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>148.10000000</t>
+          <t>188.68000000</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>299073.53972000</t>
+          <t>389668.64720000</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>1575590399999</v>
+        <v>1572998399999</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>43777241.59082360</t>
+          <t>73036074.78097270</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>111694</v>
+        <v>184562</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>159810.68936000</t>
+          <t>200247.68513000</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>23382484.67691740</t>
+          <t>37563350.67078340</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -728,52 +728,52 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1575590400000</v>
+        <v>1572998400000</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>148.11000000</t>
+          <t>188.65000000</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>149.77000000</t>
+          <t>195.09000000</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>145.74000000</t>
+          <t>187.72000000</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>148.45000000</t>
+          <t>191.16000000</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>220674.68581000</t>
+          <t>343219.92240000</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>1575676799999</v>
+        <v>1573084799999</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>32549526.39959790</t>
+          <t>65471595.20700740</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>90076</v>
+        <v>160110</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>118938.06254000</t>
+          <t>173260.42539000</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>17547902.32235480</t>
+          <t>33061667.06580340</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -787,52 +787,52 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1575676800000</v>
+        <v>1573084800000</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>148.46000000</t>
+          <t>191.16000000</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>149.49000000</t>
+          <t>192.27000000</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>146.85000000</t>
+          <t>184.59000000</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>147.14000000</t>
+          <t>186.68000000</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>140471.68588000</t>
+          <t>309882.08206000</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>1575763199999</v>
+        <v>1573171199999</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>20799551.34569560</t>
+          <t>58150631.27682950</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>70677</v>
+        <v>152881</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>73739.81386000</t>
+          <t>155433.46587000</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>10919841.57771310</t>
+          <t>29169549.29944800</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -846,52 +846,52 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1575763200000</v>
+        <v>1573171200000</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>147.16000000</t>
+          <t>186.67000000</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>151.62000000</t>
+          <t>188.26000000</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>146.11000000</t>
+          <t>181.41000000</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>150.44000000</t>
+          <t>183.74000000</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>205301.60260000</t>
+          <t>365029.75027000</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>1575849599999</v>
+        <v>1573257599999</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>30606289.28539150</t>
+          <t>67305417.40505750</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>79766</v>
+        <v>167904</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>113946.96048000</t>
+          <t>175732.31788000</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>16985317.52759580</t>
+          <t>32419070.55804890</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -905,52 +905,52 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1575849600000</v>
+        <v>1573257600000</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>150.44000000</t>
+          <t>183.71000000</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>151.19000000</t>
+          <t>185.79000000</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>146.56000000</t>
+          <t>182.63000000</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>147.38000000</t>
+          <t>184.89000000</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>243775.99249000</t>
+          <t>192073.38044000</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>1575935999999</v>
+        <v>1573343999999</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>36345702.34808850</t>
+          <t>35441967.76569950</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>92204</v>
+        <v>112521</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>113225.94088000</t>
+          <t>97836.42113000</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>16892414.52102660</t>
+          <t>18053843.37560730</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -964,52 +964,52 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1575936000000</v>
+        <v>1573344000000</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>147.40000000</t>
+          <t>184.86000000</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>148.57000000</t>
+          <t>191.58000000</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>143.81000000</t>
+          <t>183.30000000</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>145.56000000</t>
+          <t>188.96000000</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>203215.84937000</t>
+          <t>274940.53448000</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>1576022399999</v>
+        <v>1573430399999</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>29746845.43242870</t>
+          <t>51648623.28633990</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>85725</v>
+        <v>133008</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>96914.54456000</t>
+          <t>139412.49207000</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>14189982.05386240</t>
+          <t>26196034.43765130</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1023,52 +1023,52 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>1576022400000</v>
+        <v>1573430400000</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>145.53000000</t>
+          <t>188.96000000</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>146.34000000</t>
+          <t>190.19000000</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>142.12000000</t>
+          <t>184.06000000</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>143.39000000</t>
+          <t>184.98000000</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>157843.10484000</t>
+          <t>255579.93429000</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>1576108799999</v>
+        <v>1573516799999</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>22772651.16812890</t>
+          <t>47746876.45656240</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>69834</v>
+        <v>128079</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>82484.40373000</t>
+          <t>125060.86932000</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>11897456.58801180</t>
+          <t>23366849.50463640</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -1082,52 +1082,52 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1576108800000</v>
+        <v>1573516800000</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>143.41000000</t>
+          <t>184.98000000</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>145.85000000</t>
+          <t>187.65000000</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>139.24000000</t>
+          <t>182.41000000</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>144.87000000</t>
+          <t>187.09000000</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>261615.30437000</t>
+          <t>256782.63119000</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>1576195199999</v>
+        <v>1573603199999</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>37425277.03812350</t>
+          <t>47636043.35288470</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>99231</v>
+        <v>124488</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>127845.69433000</t>
+          <t>130189.09727000</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>18297930.21017830</t>
+          <t>24161522.42526670</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
@@ -1141,52 +1141,52 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1576195200000</v>
+        <v>1573603200000</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>144.87000000</t>
+          <t>187.09000000</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>146.00000000</t>
+          <t>189.66000000</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>142.80000000</t>
+          <t>185.30000000</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>144.80000000</t>
+          <t>188.11000000</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>160695.18556000</t>
+          <t>197273.84001000</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>1576281599999</v>
+        <v>1573689599999</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>23203419.96161870</t>
+          <t>36936429.93594350</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>90805</v>
+        <v>89631</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>82252.75063000</t>
+          <t>101255.98817000</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>11879184.41045830</t>
+          <t>18965818.25351880</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -1200,52 +1200,52 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>1576281600000</v>
+        <v>1573689600000</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>144.80000000</t>
+          <t>188.07000000</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>145.07000000</t>
+          <t>188.72000000</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>141.18000000</t>
+          <t>183.34000000</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>141.79000000</t>
+          <t>184.92000000</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>126232.59201000</t>
+          <t>245505.29971000</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>1576367999999</v>
+        <v>1573775999999</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>18027581.35954590</t>
+          <t>45523714.09855510</t>
         </is>
       </c>
       <c r="J15" t="n">
-        <v>76951</v>
+        <v>114266</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>59729.52052000</t>
+          <t>117241.99539000</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>8537450.10787950</t>
+          <t>21743851.27655660</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1259,55 +1259,1825 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
+        <v>1573776000000</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>184.93000000</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>186.70000000</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>177.67000000</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>180.00000000</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>407466.78964000</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>1573862399999</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>74217250.17271870</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>156868</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>196587.25275000</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>35827558.08033390</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1573862400000</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>179.99000000</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>183.46000000</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>179.30000000</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>182.37000000</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>172801.52576000</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>1573948799999</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>31378510.01538970</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>89596</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>86531.48564000</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>15713912.23090380</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1573948800000</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>182.37000000</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>186.09000000</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>180.00000000</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>183.82000000</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>198892.43720000</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>1574035199999</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>36509968.69910130</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>93753</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>99564.29673000</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>18284470.26124200</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1574035200000</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>183.82000000</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>184.06000000</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>175.01000000</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>178.20000000</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>293551.23632000</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>1574121599999</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>52985734.28078390</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>131823</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>134230.72271000</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>24254035.07827020</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1574121600000</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>178.20000000</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>178.52000000</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>172.65000000</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>175.94000000</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>275886.64110000</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>1574207999999</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>48414106.95693360</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>125824</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>138098.32741000</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>24234932.99839650</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1574208000000</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>175.93000000</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>177.41000000</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>173.50000000</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>174.72000000</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>216315.93309000</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>1574294399999</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>38001672.19309860</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>106534</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>105958.65927000</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>18616351.33195330</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1574294400000</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>174.75000000</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>175.85000000</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>157.26000000</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>161.01000000</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>473895.92992000</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>1574380799999</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>78641896.23038060</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>178521</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>234632.37028000</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>38906646.50159150</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1574380800000</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>161.02000000</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>162.79000000</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>138.00000000</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>149.56000000</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>977977.23794000</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>1574467199999</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>147595324.56439290</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>324167</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>460516.29463000</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>69562234.11476300</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1574467200000</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>149.55000000</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>154.33000000</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>146.11000000</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>151.84000000</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>369721.09960000</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>1574553599999</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>55595157.56404240</t>
+        </is>
+      </c>
+      <c r="J24" t="n">
+        <v>177816</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>188200.09056000</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>28306514.67695320</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1574553600000</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>151.84000000</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>152.86000000</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>138.62000000</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>139.96000000</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>352319.21558000</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>1574639999999</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>51503705.17773920</t>
+        </is>
+      </c>
+      <c r="J25" t="n">
+        <v>158774</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>169721.62425000</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>24806572.10681470</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1574640000000</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>139.99000000</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>151.50000000</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>131.45000000</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>145.69000000</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>749675.41303000</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>1574726399999</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>106186791.33716510</t>
+        </is>
+      </c>
+      <c r="J26" t="n">
+        <v>238649</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>369097.78378000</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>52341190.61922980</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1574726400000</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>145.81000000</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>149.97000000</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>143.37000000</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>147.47000000</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>354023.04298000</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>1574812799999</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>51873405.03929090</t>
+        </is>
+      </c>
+      <c r="J27" t="n">
+        <v>132207</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>172671.00371000</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>25305494.21800260</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1574812800000</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>147.47000000</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>155.54000000</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>140.84000000</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>152.62000000</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>564796.42840000</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>1574899199999</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>83505998.05488960</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
+        <v>192325</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>290667.89068000</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>43041430.88305020</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1574899200000</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>152.61000000</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>154.63000000</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>149.09000000</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>150.72000000</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>317714.56326000</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>1574985599999</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>48324220.62056190</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
+        <v>124573</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>158837.00332000</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>24159931.80938630</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1574985600000</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>150.69000000</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>157.60000000</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>150.23000000</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>154.57000000</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>328712.25558000</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>1575071999999</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>50649319.12094730</t>
+        </is>
+      </c>
+      <c r="J30" t="n">
+        <v>129774</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>171812.20099000</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>26479251.48421680</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1575072000000</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>154.54000000</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>155.25000000</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>149.70000000</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>151.37000000</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>226863.41299000</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>1575158399999</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>34617912.17868860</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
+        <v>96632</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>115076.90179000</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>17567465.07492850</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1575158400000</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>151.43000000</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>152.49000000</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>145.79000000</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>150.73000000</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>344178.14088000</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>1575244799999</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>51148792.08299820</t>
+        </is>
+      </c>
+      <c r="J32" t="n">
+        <v>125550</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>172849.45417000</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>25693814.94443980</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1575244800000</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>150.72000000</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>151.42000000</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>146.71000000</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>148.65000000</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>233839.09730000</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>1575331199999</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>34768563.47186470</t>
+        </is>
+      </c>
+      <c r="J33" t="n">
+        <v>107070</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>114158.87515000</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>16974888.53770170</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>1575331200000</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>148.66000000</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>149.93000000</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>145.77000000</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>147.17000000</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>196329.22503000</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>1575417599999</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>29061161.10177570</t>
+        </is>
+      </c>
+      <c r="J34" t="n">
+        <v>87660</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>100293.62450000</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>14844721.32424090</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>1575417600000</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>147.19000000</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>151.98000000</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>143.15000000</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>145.38000000</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>434430.62379000</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>1575503999999</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>63840615.24391760</t>
+        </is>
+      </c>
+      <c r="J35" t="n">
+        <v>149648</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>211404.51257000</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>31089708.18797030</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>1575504000000</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>145.45000000</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>149.02000000</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>143.64000000</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>148.10000000</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>299073.53972000</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>1575590399999</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>43777241.59082360</t>
+        </is>
+      </c>
+      <c r="J36" t="n">
+        <v>111694</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>159810.68936000</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>23382484.67691740</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>1575590400000</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>148.11000000</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>149.77000000</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>145.74000000</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>148.45000000</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>220674.68581000</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>1575676799999</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>32549526.39959790</t>
+        </is>
+      </c>
+      <c r="J37" t="n">
+        <v>90076</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>118938.06254000</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>17547902.32235480</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>1575676800000</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>148.46000000</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>149.49000000</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>146.85000000</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>147.14000000</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>140471.68588000</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>1575763199999</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>20799551.34569560</t>
+        </is>
+      </c>
+      <c r="J38" t="n">
+        <v>70677</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>73739.81386000</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>10919841.57771310</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>1575763200000</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>147.16000000</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>151.62000000</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>146.11000000</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>150.44000000</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>205301.60260000</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>1575849599999</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>30606289.28539150</t>
+        </is>
+      </c>
+      <c r="J39" t="n">
+        <v>79766</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>113946.96048000</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>16985317.52759580</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>1575849600000</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>150.44000000</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>151.19000000</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>146.56000000</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>147.38000000</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>243775.99249000</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>1575935999999</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>36345702.34808850</t>
+        </is>
+      </c>
+      <c r="J40" t="n">
+        <v>92204</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>113225.94088000</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>16892414.52102660</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1575936000000</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>147.40000000</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>148.57000000</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>143.81000000</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>145.56000000</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>203215.84937000</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>1576022399999</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>29746845.43242870</t>
+        </is>
+      </c>
+      <c r="J41" t="n">
+        <v>85725</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>96914.54456000</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>14189982.05386240</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>1576022400000</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>145.53000000</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>146.34000000</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>142.12000000</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>143.39000000</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>157843.10484000</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>1576108799999</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>22772651.16812890</t>
+        </is>
+      </c>
+      <c r="J42" t="n">
+        <v>69834</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>82484.40373000</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>11897456.58801180</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>1576108800000</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>143.41000000</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>145.85000000</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>139.24000000</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>144.87000000</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>261615.30437000</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>1576195199999</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>37425277.03812350</t>
+        </is>
+      </c>
+      <c r="J43" t="n">
+        <v>99231</v>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>127845.69433000</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>18297930.21017830</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1576195200000</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>144.87000000</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>146.00000000</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>142.80000000</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>144.80000000</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>160695.18556000</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>1576281599999</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>23203419.96161870</t>
+        </is>
+      </c>
+      <c r="J44" t="n">
+        <v>90805</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>82252.75063000</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>11879184.41045830</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>1576281600000</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>144.80000000</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>145.07000000</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>141.18000000</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>141.79000000</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>126232.59201000</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>1576367999999</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>18027581.35954590</t>
+        </is>
+      </c>
+      <c r="J45" t="n">
+        <v>76951</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>59729.52052000</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>8537450.10787950</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
         <v>1576368000000</v>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>141.79000000</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>144.12000000</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>139.92000000</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>143.12000000</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>87598.86053000</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>142.85000000</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>96086.09605000</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
         <v>1576454399999</v>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>12419079.42688460</t>
-        </is>
-      </c>
-      <c r="J16" t="n">
-        <v>38629</v>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>42411.59514000</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>6012998.17428740</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>13629940.76037980</t>
+        </is>
+      </c>
+      <c r="J46" t="n">
+        <v>43189</v>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>47180.03100000</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>6693421.29850030</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
modified:   binance1.py 	modified:   binance_ETHUSDT_data.csv 	modified:   binance_ETHUSDT_data.xlsx 	deleted:    ~$binance_ETHUSDT_data.xlsx
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +433,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1575158400</v>
+        <v>1575158400000</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -492,7 +492,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1575244800</v>
+        <v>1575244800000</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -551,7 +551,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1575331200</v>
+        <v>1575331200000</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -610,7 +610,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1575417600</v>
+        <v>1575417600000</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -669,7 +669,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1575504000</v>
+        <v>1575504000000</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -728,7 +728,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1575590400</v>
+        <v>1575590400000</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -787,7 +787,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1575676800</v>
+        <v>1575676800000</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -846,7 +846,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1575763200</v>
+        <v>1575763200000</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -905,7 +905,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1575849600</v>
+        <v>1575849600000</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -964,7 +964,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1575936000</v>
+        <v>1575936000000</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1023,7 +1023,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>1576022400</v>
+        <v>1576022400000</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1082,7 +1082,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1576108800</v>
+        <v>1576108800000</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1141,7 +1141,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1576195200</v>
+        <v>1576195200000</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1200,7 +1200,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>1576281600</v>
+        <v>1576281600000</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>1576368000</v>
+        <v>1576368000000</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1278,12 +1278,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>142.25000000</t>
+          <t>142.46000000</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>105242.90323000</t>
+          <t>151189.65877000</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1291,23 +1291,82 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>14935766.87971360</t>
+          <t>21495196.81888500</t>
         </is>
       </c>
       <c r="J16" t="n">
-        <v>48173</v>
+        <v>77131</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>51710.45326000</t>
+          <t>73238.69048000</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>7339705.91700970</t>
+          <t>10413387.06460380</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1576454400000</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>142.46000000</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>142.72000000</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>140.30000000</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>141.12000000</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>78497.62898000</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>1576540799999</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>11089010.61664710</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>41602</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>33864.95452000</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>4785822.81632040</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
modified:   binance1.py 	modified:   binance_ETHUSDT_data.csv 	modified:   binance_ETHUSDT_data.xlsx 	new file:   ~$binance_ETHUSDT_data.xlsx
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -1337,12 +1337,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>141.12000000</t>
+          <t>142.22000000</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>78497.62898000</t>
+          <t>97817.78584000</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -1350,20 +1350,20 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>11089010.61664710</t>
+          <t>13822150.19547320</t>
         </is>
       </c>
       <c r="J17" t="n">
-        <v>41602</v>
+        <v>48956</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>33864.95452000</t>
+          <t>45497.97767000</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>4785822.81632040</t>
+          <t>6431745.54879430</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">

</xml_diff>

<commit_message>
modified:   binance_ETHUSDT_data.csv 	modified:   binance_ETHUSDT_data.xlsx 	modified:   note.txt
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N351"/>
+  <dimension ref="A1:N352"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22788,17 +22788,17 @@
       </c>
       <c r="E351" t="inlineStr">
         <is>
-          <t>140.30000000</t>
+          <t>127.93000000</t>
         </is>
       </c>
       <c r="F351" t="inlineStr">
         <is>
-          <t>141.39000000</t>
+          <t>132.73000000</t>
         </is>
       </c>
       <c r="G351" t="inlineStr">
         <is>
-          <t>113962.59791000</t>
+          <t>471018.85942000</t>
         </is>
       </c>
       <c r="H351" t="n">
@@ -22806,20 +22806,20 @@
       </c>
       <c r="I351" t="inlineStr">
         <is>
-          <t>16111475.61180210</t>
+          <t>63632055.58494070</t>
         </is>
       </c>
       <c r="J351" t="n">
-        <v>54388</v>
+        <v>153717</v>
       </c>
       <c r="K351" t="inlineStr">
         <is>
-          <t>51865.86815000</t>
+          <t>215716.73176000</t>
         </is>
       </c>
       <c r="L351" t="inlineStr">
         <is>
-          <t>7334756.62631240</t>
+          <t>29112565.69520390</t>
         </is>
       </c>
       <c r="M351" t="inlineStr">
@@ -22830,6 +22830,70 @@
       <c r="N351" t="inlineStr">
         <is>
           <t>2019-12-16 08:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="B352" t="n">
+        <v>1576540800000</v>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>132.72000000</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>132.98000000</t>
+        </is>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>125.81000000</t>
+        </is>
+      </c>
+      <c r="F352" t="inlineStr">
+        <is>
+          <t>127.21000000</t>
+        </is>
+      </c>
+      <c r="G352" t="inlineStr">
+        <is>
+          <t>321521.58475000</t>
+        </is>
+      </c>
+      <c r="H352" t="n">
+        <v>1576627199999</v>
+      </c>
+      <c r="I352" t="inlineStr">
+        <is>
+          <t>41795752.35111230</t>
+        </is>
+      </c>
+      <c r="J352" t="n">
+        <v>110021</v>
+      </c>
+      <c r="K352" t="inlineStr">
+        <is>
+          <t>157271.64742000</t>
+        </is>
+      </c>
+      <c r="L352" t="inlineStr">
+        <is>
+          <t>20447079.79603960</t>
+        </is>
+      </c>
+      <c r="M352" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N352" t="inlineStr">
+        <is>
+          <t>2019-12-17 08:00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modified:   binance_ETHUSDT_data.csv 	modified:   binance_ETHUSDT_data.xlsx 	modified:   email_send.py
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N352"/>
+  <dimension ref="A1:N353"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22852,17 +22852,17 @@
       </c>
       <c r="E352" t="inlineStr">
         <is>
-          <t>125.81000000</t>
+          <t>119.11000000</t>
         </is>
       </c>
       <c r="F352" t="inlineStr">
         <is>
-          <t>127.21000000</t>
+          <t>121.88000000</t>
         </is>
       </c>
       <c r="G352" t="inlineStr">
         <is>
-          <t>321521.58475000</t>
+          <t>563257.36001000</t>
         </is>
       </c>
       <c r="H352" t="n">
@@ -22870,20 +22870,20 @@
       </c>
       <c r="I352" t="inlineStr">
         <is>
-          <t>41795752.35111230</t>
+          <t>71709329.26891930</t>
         </is>
       </c>
       <c r="J352" t="n">
-        <v>110021</v>
+        <v>178977</v>
       </c>
       <c r="K352" t="inlineStr">
         <is>
-          <t>157271.64742000</t>
+          <t>272414.29784000</t>
         </is>
       </c>
       <c r="L352" t="inlineStr">
         <is>
-          <t>20447079.79603960</t>
+          <t>34693963.88197660</t>
         </is>
       </c>
       <c r="M352" t="inlineStr">
@@ -22894,6 +22894,70 @@
       <c r="N352" t="inlineStr">
         <is>
           <t>2019-12-17 08:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="1" t="n">
+        <v>351</v>
+      </c>
+      <c r="B353" t="n">
+        <v>1576627200000</v>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>121.88000000</t>
+        </is>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>129.40000000</t>
+        </is>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>116.26000000</t>
+        </is>
+      </c>
+      <c r="F353" t="inlineStr">
+        <is>
+          <t>127.13000000</t>
+        </is>
+      </c>
+      <c r="G353" t="inlineStr">
+        <is>
+          <t>658610.70636000</t>
+        </is>
+      </c>
+      <c r="H353" t="n">
+        <v>1576713599999</v>
+      </c>
+      <c r="I353" t="inlineStr">
+        <is>
+          <t>81049894.51678660</t>
+        </is>
+      </c>
+      <c r="J353" t="n">
+        <v>184282</v>
+      </c>
+      <c r="K353" t="inlineStr">
+        <is>
+          <t>346880.50773000</t>
+        </is>
+      </c>
+      <c r="L353" t="inlineStr">
+        <is>
+          <t>42673127.38978000</t>
+        </is>
+      </c>
+      <c r="M353" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N353" t="inlineStr">
+        <is>
+          <t>2019-12-18 08:00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
new file:   .DS_Store 	modified:   binance_ETHUSDT_data.csv 	modified:   binance_ETHUSDT_data.xlsx 	modified:   email_send.py 	new file:   log 	new file:   run_eth.sh
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -22921,12 +22921,12 @@
       </c>
       <c r="F353" t="inlineStr">
         <is>
-          <t>127.13000000</t>
+          <t>127.08000000</t>
         </is>
       </c>
       <c r="G353" t="inlineStr">
         <is>
-          <t>658610.70636000</t>
+          <t>665126.81604000</t>
         </is>
       </c>
       <c r="H353" t="n">
@@ -22934,20 +22934,20 @@
       </c>
       <c r="I353" t="inlineStr">
         <is>
-          <t>81049894.51678660</t>
+          <t>81879125.55131180</t>
         </is>
       </c>
       <c r="J353" t="n">
-        <v>184282</v>
+        <v>187118</v>
       </c>
       <c r="K353" t="inlineStr">
         <is>
-          <t>346880.50773000</t>
+          <t>350576.88889000</t>
         </is>
       </c>
       <c r="L353" t="inlineStr">
         <is>
-          <t>42673127.38978000</t>
+          <t>43143546.22814950</t>
         </is>
       </c>
       <c r="M353" t="inlineStr">

</xml_diff>

<commit_message>
modified:   binance_ETHUSDT_data.csv 	modified:   binance_ETHUSDT_data.xlsx 	modified:   log 	modified:   note.txt
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -22921,12 +22921,12 @@
       </c>
       <c r="F353" t="inlineStr">
         <is>
-          <t>127.08000000</t>
+          <t>126.48000000</t>
         </is>
       </c>
       <c r="G353" t="inlineStr">
         <is>
-          <t>665126.81604000</t>
+          <t>669119.30798000</t>
         </is>
       </c>
       <c r="H353" t="n">
@@ -22934,20 +22934,20 @@
       </c>
       <c r="I353" t="inlineStr">
         <is>
-          <t>81879125.55131180</t>
+          <t>82385284.66629440</t>
         </is>
       </c>
       <c r="J353" t="n">
-        <v>187118</v>
+        <v>188005</v>
       </c>
       <c r="K353" t="inlineStr">
         <is>
-          <t>350576.88889000</t>
+          <t>352399.75973000</t>
         </is>
       </c>
       <c r="L353" t="inlineStr">
         <is>
-          <t>43143546.22814950</t>
+          <t>43374582.92545460</t>
         </is>
       </c>
       <c r="M353" t="inlineStr">

</xml_diff>

<commit_message>
modified:   binance_ETHUSDT_data.csv 	modified:   binance_ETHUSDT_data.xlsx 	modified:   log
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -2435,12 +2435,12 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>127.14000000</t>
+          <t>127.18000000</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>117056.20255000</t>
+          <t>117174.26783000</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -2448,20 +2448,20 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>14894050.32577060</t>
+          <t>14909067.13294150</t>
         </is>
       </c>
       <c r="J22" t="n">
-        <v>52518</v>
+        <v>52615</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>56108.69620000</t>
+          <t>56214.06181000</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>7139067.75957560</t>
+          <t>7152469.37395310</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -2470,38 +2470,38 @@
         </is>
       </c>
       <c r="N22" t="n">
-        <v>127.1399999999999</v>
+        <v>127.1799999999999</v>
       </c>
       <c r="O22" t="n">
-        <v>127.665</v>
+        <v>127.685</v>
       </c>
       <c r="P22" t="n">
-        <v>130.4685714285714</v>
+        <v>130.4742857142856</v>
       </c>
       <c r="Q22" t="n">
-        <v>138.5766666666667</v>
+        <v>138.5793333333333</v>
       </c>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="n">
-        <v>127.14</v>
+        <v>127.18</v>
       </c>
       <c r="T22" t="n">
-        <v>127.5769105669497</v>
+        <v>127.6035772336189</v>
       </c>
       <c r="U22" t="n">
-        <v>134.0794035572041</v>
+        <v>134.0857474191577</v>
       </c>
       <c r="V22" t="n">
-        <v>137.7229579217146</v>
+        <v>137.7266554124672</v>
       </c>
       <c r="W22" t="n">
-        <v>-3.643554364510464</v>
+        <v>-3.640907993309554</v>
       </c>
       <c r="X22" t="n">
-        <v>-2.396484297590332</v>
+        <v>-2.395950096212096</v>
       </c>
       <c r="Y22" t="n">
-        <v>-1.247070066920132</v>
+        <v>-1.244957897097458</v>
       </c>
       <c r="Z22" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
modified:   .DS_Store 	modified:   __pycache__/binance1.cpython-38.pyc 	modified:   binance1.py 	modified:   binance_ETHUSDT_data.csv 	modified:   binance_ETHUSDT_data.xlsx 	modified:   log 	modified:   trades_df.xlsx 	renamed:    ~$trades_df.xlsx -> ~$binance_ETHUSDT_data.xlsx
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X15"/>
+  <dimension ref="A1:X20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1629,17 +1629,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>130.87000000</t>
+          <t>126.00000000</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>133.25000000</t>
+          <t>127.80000000</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>245657.75029000</t>
+          <t>421600.75655000</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -1647,20 +1647,20 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>32680918.14505240</t>
+          <t>55501305.92012300</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>86685</v>
+        <v>145867</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>113741.05451000</t>
+          <t>194731.21180000</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>15133465.86360570</t>
+          <t>25638865.78568890</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1669,36 +1669,486 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>133.2499999999999</v>
+        <v>127.7999999999999</v>
       </c>
       <c r="N15" t="n">
-        <v>132.67</v>
+        <v>129.9450000000001</v>
       </c>
       <c r="O15" t="n">
-        <v>129.04</v>
+        <v>128.2614285714286</v>
       </c>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="n">
-        <v>133.25</v>
+        <v>127.8</v>
       </c>
       <c r="S15" t="n">
-        <v>132.3507645545611</v>
+        <v>128.7174304615879</v>
       </c>
       <c r="T15" t="n">
-        <v>132.4673963041822</v>
+        <v>131.5394353129163</v>
       </c>
       <c r="U15" t="n">
-        <v>133.9354477793955</v>
+        <v>133.3233479202179</v>
       </c>
       <c r="V15" t="n">
-        <v>-1.468051475213286</v>
+        <v>-1.783912607301687</v>
       </c>
       <c r="W15" t="n">
-        <v>-1.398837152580375</v>
+        <v>-1.464915537082233</v>
       </c>
       <c r="X15" t="n">
-        <v>-0.06921432263291183</v>
+        <v>-0.3189970702194544</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>127.80000000</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>129.69000000</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>126.61000000</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>127.75000000</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>200637.10098000</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>1577231999999</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>25667665.14201030</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>87657</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>100608.48356000</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>12872420.08887930</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>2019-12-24 08:00:00</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>127.7499999999999</v>
+      </c>
+      <c r="N16" t="n">
+        <v>127.775</v>
+      </c>
+      <c r="O16" t="n">
+        <v>129.1</v>
+      </c>
+      <c r="P16" t="n">
+        <v>134.7453333333333</v>
+      </c>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="n">
+        <v>127.75</v>
+      </c>
+      <c r="S16" t="n">
+        <v>128.0724767755814</v>
+      </c>
+      <c r="T16" t="n">
+        <v>130.9046400251341</v>
+      </c>
+      <c r="U16" t="n">
+        <v>132.720448196802</v>
+      </c>
+      <c r="V16" t="n">
+        <v>-1.815808171667896</v>
+      </c>
+      <c r="W16" t="n">
+        <v>-1.537653296387676</v>
+      </c>
+      <c r="X16" t="n">
+        <v>-0.2781548752802205</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>127.70000000</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>127.84000000</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>123.07000000</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>125.09000000</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>225004.49090000</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>1577318399999</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>28144469.16072900</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>93397</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>98563.14610000</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>12331982.19518460</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>2019-12-25 08:00:00</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
+        <v>125.0899999999999</v>
+      </c>
+      <c r="N17" t="n">
+        <v>126.42</v>
+      </c>
+      <c r="O17" t="n">
+        <v>128.0014285714286</v>
+      </c>
+      <c r="P17" t="n">
+        <v>133.3806666666667</v>
+      </c>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="n">
+        <v>125.09</v>
+      </c>
+      <c r="S17" t="n">
+        <v>126.084158879004</v>
+      </c>
+      <c r="T17" t="n">
+        <v>129.9437249151322</v>
+      </c>
+      <c r="U17" t="n">
+        <v>131.9222406327808</v>
+      </c>
+      <c r="V17" t="n">
+        <v>-1.978515717648605</v>
+      </c>
+      <c r="W17" t="n">
+        <v>-1.628379496135982</v>
+      </c>
+      <c r="X17" t="n">
+        <v>-0.3501362215126234</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>125.09000000</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>132.26000000</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>124.32000000</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>125.58000000</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>274986.52097000</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>1577404799999</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>34943780.90920390</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>103034</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>128410.01213000</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>16332907.92974440</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>2019-12-26 08:00:00</t>
+        </is>
+      </c>
+      <c r="M18" t="n">
+        <v>125.5799999999999</v>
+      </c>
+      <c r="N18" t="n">
+        <v>125.335</v>
+      </c>
+      <c r="O18" t="n">
+        <v>127.6414285714286</v>
+      </c>
+      <c r="P18" t="n">
+        <v>132.1933333333333</v>
+      </c>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="n">
+        <v>125.58</v>
+      </c>
+      <c r="S18" t="n">
+        <v>125.7480529570654</v>
+      </c>
+      <c r="T18" t="n">
+        <v>129.2307215690578</v>
+      </c>
+      <c r="U18" t="n">
+        <v>131.2784478225959</v>
+      </c>
+      <c r="V18" t="n">
+        <v>-2.047726253538031</v>
+      </c>
+      <c r="W18" t="n">
+        <v>-1.714180924009384</v>
+      </c>
+      <c r="X18" t="n">
+        <v>-0.3335453295286464</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>125.58000000</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>127.10000000</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>121.91000000</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>126.29000000</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>240012.37451000</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>1577491199999</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>30020098.88913110</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>102142</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>115839.00216000</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>14500702.34866460</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>2019-12-27 08:00:00</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
+        <v>126.2899999999999</v>
+      </c>
+      <c r="N19" t="n">
+        <v>125.935</v>
+      </c>
+      <c r="O19" t="n">
+        <v>127.37</v>
+      </c>
+      <c r="P19" t="n">
+        <v>130.9546666666667</v>
+      </c>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="n">
+        <v>126.29</v>
+      </c>
+      <c r="S19" t="n">
+        <v>126.109350986621</v>
+      </c>
+      <c r="T19" t="n">
+        <v>128.7547713720667</v>
+      </c>
+      <c r="U19" t="n">
+        <v>130.7855979726117</v>
+      </c>
+      <c r="V19" t="n">
+        <v>-2.030826600544998</v>
+      </c>
+      <c r="W19" t="n">
+        <v>-1.778671824090809</v>
+      </c>
+      <c r="X19" t="n">
+        <v>-0.2521547764541889</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>126.28000000</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>128.59000000</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>125.84000000</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>127.28000000</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>77413.69234000</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>1577577599999</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>9862089.16080160</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>34300</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>39247.83833000</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>5001388.97613230</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>2019-12-28 08:00:00</t>
+        </is>
+      </c>
+      <c r="M20" t="n">
+        <v>127.2799999999999</v>
+      </c>
+      <c r="N20" t="n">
+        <v>126.7850000000001</v>
+      </c>
+      <c r="O20" t="n">
+        <v>127.4114285714286</v>
+      </c>
+      <c r="P20" t="n">
+        <v>129.7866666666667</v>
+      </c>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="n">
+        <v>127.28</v>
+      </c>
+      <c r="S20" t="n">
+        <v>126.8897836628785</v>
+      </c>
+      <c r="T20" t="n">
+        <v>128.5179772421101</v>
+      </c>
+      <c r="U20" t="n">
+        <v>130.4476076024285</v>
+      </c>
+      <c r="V20" t="n">
+        <v>-1.929630360318413</v>
+      </c>
+      <c r="W20" t="n">
+        <v>-1.809305001955259</v>
+      </c>
+      <c r="X20" t="n">
+        <v>-0.1203253583631536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   .DS_Store 	modified:   __pycache__/binance1.cpython-38.pyc 	modified:   binance1.py 	modified:   binance_ETHUSDT_data.csv 	modified:   binance_ETHUSDT_data.xlsx 	new file:   data.txt 	modified:   email_send.py 	new file:   email_send_signal.txt 	modified:   log 	modified:   trades_df.xlsx
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -2082,12 +2082,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>127.28000000</t>
+          <t>127.19000000</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>77413.69234000</t>
+          <t>84488.07392000</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -2095,20 +2095,20 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>9862089.16080160</t>
+          <t>10762496.22348290</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>34300</v>
+        <v>37823</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>39247.83833000</t>
+          <t>43243.29299000</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>5001388.97613230</t>
+          <t>5510042.32479330</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -2117,38 +2117,38 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>127.2799999999999</v>
+        <v>127.1899999999999</v>
       </c>
       <c r="N20" t="n">
-        <v>126.7850000000001</v>
+        <v>126.74</v>
       </c>
       <c r="O20" t="n">
-        <v>127.4114285714286</v>
+        <v>127.3985714285714</v>
       </c>
       <c r="P20" t="n">
-        <v>129.7866666666667</v>
+        <v>129.7806666666667</v>
       </c>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="n">
-        <v>127.28</v>
+        <v>127.19</v>
       </c>
       <c r="S20" t="n">
-        <v>126.8897836628785</v>
+        <v>126.8297836628268</v>
       </c>
       <c r="T20" t="n">
-        <v>128.5179772421101</v>
+        <v>128.5035265468364</v>
       </c>
       <c r="U20" t="n">
-        <v>130.4476076024285</v>
+        <v>130.4389303001382</v>
       </c>
       <c r="V20" t="n">
-        <v>-1.929630360318413</v>
+        <v>-1.935403753301813</v>
       </c>
       <c r="W20" t="n">
-        <v>-1.809305001955259</v>
+        <v>-1.810476564548283</v>
       </c>
       <c r="X20" t="n">
-        <v>-0.1203253583631536</v>
+        <v>-0.1249271887535299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   binance_ETHUSDT_data.csv 	modified:   binance_ETHUSDT_data.xlsx 	modified:   email_send.py 	modified:   log 	modified:   trades_df.xlsx
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -2082,12 +2082,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>127.19000000</t>
+          <t>127.12000000</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>84488.07392000</t>
+          <t>84693.74392000</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -2095,20 +2095,20 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>10762496.22348290</t>
+          <t>10788650.59353520</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>37823</v>
+        <v>37982</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>43243.29299000</t>
+          <t>43316.73631000</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>5510042.32479330</t>
+          <t>5519382.19591250</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -2117,38 +2117,38 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>127.1899999999999</v>
+        <v>127.1199999999999</v>
       </c>
       <c r="N20" t="n">
-        <v>126.74</v>
+        <v>126.7050000000001</v>
       </c>
       <c r="O20" t="n">
-        <v>127.3985714285714</v>
+        <v>127.3885714285714</v>
       </c>
       <c r="P20" t="n">
-        <v>129.7806666666667</v>
+        <v>129.776</v>
       </c>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="n">
-        <v>127.19</v>
+        <v>127.12</v>
       </c>
       <c r="S20" t="n">
-        <v>126.8297836628268</v>
+        <v>126.78311699612</v>
       </c>
       <c r="T20" t="n">
-        <v>128.5035265468364</v>
+        <v>128.4922871171791</v>
       </c>
       <c r="U20" t="n">
-        <v>130.4389303001382</v>
+        <v>130.4321812872458</v>
       </c>
       <c r="V20" t="n">
-        <v>-1.935403753301813</v>
+        <v>-1.939894170066708</v>
       </c>
       <c r="W20" t="n">
-        <v>-1.810476564548283</v>
+        <v>-1.811387779898418</v>
       </c>
       <c r="X20" t="n">
-        <v>-0.1249271887535299</v>
+        <v>-0.1285063901682899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish the email send content
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -2082,12 +2082,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>127.24000000</t>
+          <t>127.42000000</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>84986.85020000</t>
+          <t>85596.04072000</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -2095,20 +2095,20 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>10825933.45785530</t>
+          <t>10903507.61611180</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>38188</v>
+        <v>38744</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>43438.08967000</t>
+          <t>43752.55114000</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>5534819.02770030</t>
+          <t>5574866.68277130</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -2117,38 +2117,38 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>127.2399999999999</v>
+        <v>127.4199999999999</v>
       </c>
       <c r="N20" t="n">
-        <v>126.765</v>
+        <v>126.855</v>
       </c>
       <c r="O20" t="n">
-        <v>127.4057142857143</v>
+        <v>127.4314285714286</v>
       </c>
       <c r="P20" t="n">
-        <v>129.784</v>
+        <v>129.796</v>
       </c>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="n">
-        <v>127.24</v>
+        <v>127.42</v>
       </c>
       <c r="S20" t="n">
-        <v>126.8631169961889</v>
+        <v>126.9831169962921</v>
       </c>
       <c r="T20" t="n">
-        <v>128.5115547108773</v>
+        <v>128.5404561014247</v>
       </c>
       <c r="U20" t="n">
-        <v>130.4437510236328</v>
+        <v>130.4611056282133</v>
       </c>
       <c r="V20" t="n">
-        <v>-1.93219631275548</v>
+        <v>-1.920649526788651</v>
       </c>
       <c r="W20" t="n">
-        <v>-1.809825696441048</v>
+        <v>-1.807482571254994</v>
       </c>
       <c r="X20" t="n">
-        <v>-0.122370616314432</v>
+        <v>-0.1131669555336565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust the mail font
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -504,12 +504,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>128.15000000</t>
+          <t>128.20000000</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>44548.67679000</t>
+          <t>44560.50574000</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -517,20 +517,20 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>5707923.32374280</t>
+          <t>5709439.42501910</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>22594</v>
+        <v>22611</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>21717.21714000</t>
+          <t>21721.68202000</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2782400.50389010</t>
+          <t>2782972.72016410</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -539,23 +539,23 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>128.15</v>
+        <v>128.2</v>
       </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="n">
-        <v>128.15</v>
+        <v>128.2</v>
       </c>
       <c r="S2" t="n">
-        <v>128.15</v>
+        <v>128.2</v>
       </c>
       <c r="T2" t="n">
-        <v>128.15</v>
+        <v>128.2</v>
       </c>
       <c r="U2" t="n">
-        <v>128.15</v>
+        <v>128.2</v>
       </c>
       <c r="V2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
add the file in attachments and adjust the email notify shell script
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -79892,12 +79892,12 @@
       </c>
       <c r="E866" t="inlineStr">
         <is>
-          <t>128.40000000</t>
+          <t>128.38000000</t>
         </is>
       </c>
       <c r="F866" t="inlineStr">
         <is>
-          <t>50706.12794000</t>
+          <t>50716.25614000</t>
         </is>
       </c>
       <c r="G866" t="n">
@@ -79905,20 +79905,20 @@
       </c>
       <c r="H866" t="inlineStr">
         <is>
-          <t>6497705.56211640</t>
+          <t>6499005.89037800</t>
         </is>
       </c>
       <c r="I866" t="n">
-        <v>25421</v>
+        <v>25443</v>
       </c>
       <c r="J866" t="inlineStr">
         <is>
-          <t>24599.67506000</t>
+          <t>24604.18338000</t>
         </is>
       </c>
       <c r="K866" t="inlineStr">
         <is>
-          <t>3152026.04683560</t>
+          <t>3152604.85488250</t>
         </is>
       </c>
       <c r="L866" t="inlineStr">
@@ -79927,40 +79927,40 @@
         </is>
       </c>
       <c r="M866" t="n">
-        <v>128.3999999999992</v>
+        <v>128.3799999999992</v>
       </c>
       <c r="N866" t="n">
-        <v>128.2550000000003</v>
+        <v>128.2450000000002</v>
       </c>
       <c r="O866" t="n">
-        <v>127.002857142856</v>
+        <v>126.9999999999988</v>
       </c>
       <c r="P866" t="n">
-        <v>128.9493333333337</v>
+        <v>128.9480000000003</v>
       </c>
       <c r="Q866" t="n">
-        <v>137.9820000000003</v>
+        <v>137.9813333333336</v>
       </c>
       <c r="R866" t="n">
-        <v>128.4</v>
+        <v>128.38</v>
       </c>
       <c r="S866" t="n">
-        <v>128.0810390048117</v>
+        <v>128.0677056714783</v>
       </c>
       <c r="T866" t="n">
-        <v>129.366831608848</v>
+        <v>129.3637546857711</v>
       </c>
       <c r="U866" t="n">
-        <v>135.9646185085518</v>
+        <v>135.9631370270703</v>
       </c>
       <c r="V866" t="n">
-        <v>-6.597786899703777</v>
+        <v>-6.599382341299219</v>
       </c>
       <c r="W866" t="n">
-        <v>-7.365345204108266</v>
+        <v>-7.365664292427354</v>
       </c>
       <c r="X866" t="n">
-        <v>0.7675583044044885</v>
+        <v>0.7662819511281356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add the buy sell text in email
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -79892,12 +79892,12 @@
       </c>
       <c r="E866" t="inlineStr">
         <is>
-          <t>128.38000000</t>
+          <t>128.30000000</t>
         </is>
       </c>
       <c r="F866" t="inlineStr">
         <is>
-          <t>50716.25614000</t>
+          <t>51156.56681000</t>
         </is>
       </c>
       <c r="G866" t="n">
@@ -79905,20 +79905,20 @@
       </c>
       <c r="H866" t="inlineStr">
         <is>
-          <t>6499005.89037800</t>
+          <t>6555532.51073730</t>
         </is>
       </c>
       <c r="I866" t="n">
-        <v>25443</v>
+        <v>25673</v>
       </c>
       <c r="J866" t="inlineStr">
         <is>
-          <t>24604.18338000</t>
+          <t>24733.77306000</t>
         </is>
       </c>
       <c r="K866" t="inlineStr">
         <is>
-          <t>3152604.85488250</t>
+          <t>3169244.28219340</t>
         </is>
       </c>
       <c r="L866" t="inlineStr">
@@ -79927,40 +79927,40 @@
         </is>
       </c>
       <c r="M866" t="n">
-        <v>128.3799999999992</v>
+        <v>128.2999999999992</v>
       </c>
       <c r="N866" t="n">
-        <v>128.2450000000002</v>
+        <v>128.2050000000002</v>
       </c>
       <c r="O866" t="n">
-        <v>126.9999999999988</v>
+        <v>126.9885714285703</v>
       </c>
       <c r="P866" t="n">
-        <v>128.9480000000003</v>
+        <v>128.942666666667</v>
       </c>
       <c r="Q866" t="n">
-        <v>137.9813333333336</v>
+        <v>137.9786666666669</v>
       </c>
       <c r="R866" t="n">
-        <v>128.38</v>
+        <v>128.3</v>
       </c>
       <c r="S866" t="n">
-        <v>128.0677056714783</v>
+        <v>128.014372338145</v>
       </c>
       <c r="T866" t="n">
-        <v>129.3637546857711</v>
+        <v>129.3514469934634</v>
       </c>
       <c r="U866" t="n">
-        <v>135.9631370270703</v>
+        <v>135.9572111011443</v>
       </c>
       <c r="V866" t="n">
-        <v>-6.599382341299219</v>
+        <v>-6.605764107680983</v>
       </c>
       <c r="W866" t="n">
-        <v>-7.365664292427354</v>
+        <v>-7.366940645703707</v>
       </c>
       <c r="X866" t="n">
-        <v>0.7662819511281356</v>
+        <v>0.761176538022724</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   binance_ETHUSDT_data.csv 	modified:   binance_ETHUSDT_data.xlsx 	modified:   log 	modified:   trade_details.csv 	modified:   trades_df.csv
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -79892,12 +79892,12 @@
       </c>
       <c r="E866" t="inlineStr">
         <is>
-          <t>131.81000000</t>
+          <t>131.82000000</t>
         </is>
       </c>
       <c r="F866" t="inlineStr">
         <is>
-          <t>128183.15096000</t>
+          <t>128356.40578000</t>
         </is>
       </c>
       <c r="G866" t="n">
@@ -79905,20 +79905,20 @@
       </c>
       <c r="H866" t="inlineStr">
         <is>
-          <t>16605614.21490530</t>
+          <t>16628454.43571890</t>
         </is>
       </c>
       <c r="I866" t="n">
-        <v>54010</v>
+        <v>54087</v>
       </c>
       <c r="J866" t="inlineStr">
         <is>
-          <t>63790.45804000</t>
+          <t>63890.11150000</t>
         </is>
       </c>
       <c r="K866" t="inlineStr">
         <is>
-          <t>8265696.86369070</t>
+          <t>8278834.35856570</t>
         </is>
       </c>
       <c r="L866" t="inlineStr">
@@ -79927,40 +79927,40 @@
         </is>
       </c>
       <c r="M866" t="n">
-        <v>131.8099999999992</v>
+        <v>131.8199999999992</v>
       </c>
       <c r="N866" t="n">
-        <v>129.9600000000002</v>
+        <v>129.9650000000002</v>
       </c>
       <c r="O866" t="n">
-        <v>127.4899999999989</v>
+        <v>127.4914285714274</v>
       </c>
       <c r="P866" t="n">
-        <v>129.176666666667</v>
+        <v>129.1773333333337</v>
       </c>
       <c r="Q866" t="n">
-        <v>138.0956666666669</v>
+        <v>138.0960000000003</v>
       </c>
       <c r="R866" t="n">
-        <v>131.81</v>
+        <v>131.82</v>
       </c>
       <c r="S866" t="n">
-        <v>130.354372338145</v>
+        <v>130.3610390048117</v>
       </c>
       <c r="T866" t="n">
-        <v>129.8914469934633</v>
+        <v>129.8929854550018</v>
       </c>
       <c r="U866" t="n">
-        <v>136.2172111011443</v>
+        <v>136.2179518418851</v>
       </c>
       <c r="V866" t="n">
-        <v>-6.325764107680982</v>
+        <v>-6.32496638688329</v>
       </c>
       <c r="W866" t="n">
-        <v>-7.310940645703707</v>
+        <v>-7.310781101544168</v>
       </c>
       <c r="X866" t="n">
-        <v>0.9851765380227251</v>
+        <v>0.9858147146608784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust the send mail conditions
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X866"/>
+  <dimension ref="A1:X867"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -79882,7 +79882,7 @@
       </c>
       <c r="C866" t="inlineStr">
         <is>
-          <t>131.93000000</t>
+          <t>138.07000000</t>
         </is>
       </c>
       <c r="D866" t="inlineStr">
@@ -79892,12 +79892,12 @@
       </c>
       <c r="E866" t="inlineStr">
         <is>
-          <t>131.82000000</t>
+          <t>134.36000000</t>
         </is>
       </c>
       <c r="F866" t="inlineStr">
         <is>
-          <t>128356.40578000</t>
+          <t>316347.26666000</t>
         </is>
       </c>
       <c r="G866" t="n">
@@ -79905,20 +79905,20 @@
       </c>
       <c r="H866" t="inlineStr">
         <is>
-          <t>16628454.43571890</t>
+          <t>41893078.36221210</t>
         </is>
       </c>
       <c r="I866" t="n">
-        <v>54087</v>
+        <v>115498</v>
       </c>
       <c r="J866" t="inlineStr">
         <is>
-          <t>63890.11150000</t>
+          <t>154769.98070000</t>
         </is>
       </c>
       <c r="K866" t="inlineStr">
         <is>
-          <t>8278834.35856570</t>
+          <t>20495780.18127650</t>
         </is>
       </c>
       <c r="L866" t="inlineStr">
@@ -79927,40 +79927,132 @@
         </is>
       </c>
       <c r="M866" t="n">
-        <v>131.8199999999992</v>
+        <v>134.3599999999992</v>
       </c>
       <c r="N866" t="n">
-        <v>129.9650000000002</v>
+        <v>131.2350000000002</v>
       </c>
       <c r="O866" t="n">
-        <v>127.4914285714274</v>
+        <v>127.8542857142846</v>
       </c>
       <c r="P866" t="n">
-        <v>129.1773333333337</v>
+        <v>129.346666666667</v>
       </c>
       <c r="Q866" t="n">
-        <v>138.0960000000003</v>
+        <v>138.1806666666669</v>
       </c>
       <c r="R866" t="n">
-        <v>131.82</v>
+        <v>134.36</v>
       </c>
       <c r="S866" t="n">
-        <v>130.3610390048117</v>
+        <v>132.054372338145</v>
       </c>
       <c r="T866" t="n">
-        <v>129.8929854550018</v>
+        <v>130.283754685771</v>
       </c>
       <c r="U866" t="n">
-        <v>136.2179518418851</v>
+        <v>136.4060999900333</v>
       </c>
       <c r="V866" t="n">
-        <v>-6.32496638688329</v>
+        <v>-6.122345304262211</v>
       </c>
       <c r="W866" t="n">
-        <v>-7.310781101544168</v>
+        <v>-7.270256885019952</v>
       </c>
       <c r="X866" t="n">
-        <v>0.9858147146608784</v>
+        <v>1.147911580757741</v>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" s="1" t="n">
+        <v>865</v>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>134.36000000</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>136.24000000</t>
+        </is>
+      </c>
+      <c r="D867" t="inlineStr">
+        <is>
+          <t>130.33000000</t>
+        </is>
+      </c>
+      <c r="E867" t="inlineStr">
+        <is>
+          <t>130.70000000</t>
+        </is>
+      </c>
+      <c r="F867" t="inlineStr">
+        <is>
+          <t>236283.25464000</t>
+        </is>
+      </c>
+      <c r="G867" t="n">
+        <v>1577750399999</v>
+      </c>
+      <c r="H867" t="inlineStr">
+        <is>
+          <t>31593668.97287620</t>
+        </is>
+      </c>
+      <c r="I867" t="n">
+        <v>70337</v>
+      </c>
+      <c r="J867" t="inlineStr">
+        <is>
+          <t>115196.20005000</t>
+        </is>
+      </c>
+      <c r="K867" t="inlineStr">
+        <is>
+          <t>15407529.78767640</t>
+        </is>
+      </c>
+      <c r="L867" t="inlineStr">
+        <is>
+          <t>2019-12-30 08:00:00</t>
+        </is>
+      </c>
+      <c r="M867" t="n">
+        <v>130.6999999999992</v>
+      </c>
+      <c r="N867" t="n">
+        <v>132.5300000000002</v>
+      </c>
+      <c r="O867" t="n">
+        <v>128.2685714285703</v>
+      </c>
+      <c r="P867" t="n">
+        <v>128.562666666667</v>
+      </c>
+      <c r="Q867" t="n">
+        <v>137.4916666666669</v>
+      </c>
+      <c r="R867" t="n">
+        <v>130.7</v>
+      </c>
+      <c r="S867" t="n">
+        <v>131.1514574460483</v>
+      </c>
+      <c r="T867" t="n">
+        <v>130.3477924264216</v>
+      </c>
+      <c r="U867" t="n">
+        <v>135.9834259166975</v>
+      </c>
+      <c r="V867" t="n">
+        <v>-5.635633490275808</v>
+      </c>
+      <c r="W867" t="n">
+        <v>-6.943332206071124</v>
+      </c>
+      <c r="X867" t="n">
+        <v>1.307698715795317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add the attach in buy sell signal email
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -79984,12 +79984,12 @@
       </c>
       <c r="E867" t="inlineStr">
         <is>
-          <t>130.70000000</t>
+          <t>130.47000000</t>
         </is>
       </c>
       <c r="F867" t="inlineStr">
         <is>
-          <t>236283.25464000</t>
+          <t>236795.09181000</t>
         </is>
       </c>
       <c r="G867" t="n">
@@ -79997,20 +79997,20 @@
       </c>
       <c r="H867" t="inlineStr">
         <is>
-          <t>31593668.97287620</t>
+          <t>31660490.79451830</t>
         </is>
       </c>
       <c r="I867" t="n">
-        <v>70337</v>
+        <v>70476</v>
       </c>
       <c r="J867" t="inlineStr">
         <is>
-          <t>115196.20005000</t>
+          <t>115469.68419000</t>
         </is>
       </c>
       <c r="K867" t="inlineStr">
         <is>
-          <t>15407529.78767640</t>
+          <t>15443235.54415320</t>
         </is>
       </c>
       <c r="L867" t="inlineStr">
@@ -80019,40 +80019,40 @@
         </is>
       </c>
       <c r="M867" t="n">
-        <v>130.6999999999992</v>
+        <v>130.4699999999992</v>
       </c>
       <c r="N867" t="n">
-        <v>132.5300000000002</v>
+        <v>132.4150000000002</v>
       </c>
       <c r="O867" t="n">
-        <v>128.2685714285703</v>
+        <v>128.2357142857131</v>
       </c>
       <c r="P867" t="n">
-        <v>128.562666666667</v>
+        <v>128.5473333333337</v>
       </c>
       <c r="Q867" t="n">
-        <v>137.4916666666669</v>
+        <v>137.4840000000003</v>
       </c>
       <c r="R867" t="n">
-        <v>130.7</v>
+        <v>130.47</v>
       </c>
       <c r="S867" t="n">
-        <v>131.1514574460483</v>
+        <v>130.998124112715</v>
       </c>
       <c r="T867" t="n">
-        <v>130.3477924264216</v>
+        <v>130.312407811037</v>
       </c>
       <c r="U867" t="n">
-        <v>135.9834259166975</v>
+        <v>135.9663888796604</v>
       </c>
       <c r="V867" t="n">
-        <v>-5.635633490275808</v>
+        <v>-5.653981068623381</v>
       </c>
       <c r="W867" t="n">
-        <v>-6.943332206071124</v>
+        <v>-6.947001721740639</v>
       </c>
       <c r="X867" t="n">
-        <v>1.307698715795317</v>
+        <v>1.293020653117258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add the EMA in email
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -79979,17 +79979,17 @@
       </c>
       <c r="D867" t="inlineStr">
         <is>
-          <t>130.33000000</t>
+          <t>130.30000000</t>
         </is>
       </c>
       <c r="E867" t="inlineStr">
         <is>
-          <t>130.47000000</t>
+          <t>131.29000000</t>
         </is>
       </c>
       <c r="F867" t="inlineStr">
         <is>
-          <t>236795.09181000</t>
+          <t>267805.58315000</t>
         </is>
       </c>
       <c r="G867" t="n">
@@ -79997,20 +79997,20 @@
       </c>
       <c r="H867" t="inlineStr">
         <is>
-          <t>31660490.79451830</t>
+          <t>35717036.53360180</t>
         </is>
       </c>
       <c r="I867" t="n">
-        <v>70476</v>
+        <v>80990</v>
       </c>
       <c r="J867" t="inlineStr">
         <is>
-          <t>115469.68419000</t>
+          <t>128942.90379000</t>
         </is>
       </c>
       <c r="K867" t="inlineStr">
         <is>
-          <t>15443235.54415320</t>
+          <t>17205475.24753970</t>
         </is>
       </c>
       <c r="L867" t="inlineStr">
@@ -80019,40 +80019,40 @@
         </is>
       </c>
       <c r="M867" t="n">
-        <v>130.4699999999992</v>
+        <v>131.2899999999992</v>
       </c>
       <c r="N867" t="n">
-        <v>132.4150000000002</v>
+        <v>132.8250000000002</v>
       </c>
       <c r="O867" t="n">
-        <v>128.2357142857131</v>
+        <v>128.352857142856</v>
       </c>
       <c r="P867" t="n">
-        <v>128.5473333333337</v>
+        <v>128.6020000000003</v>
       </c>
       <c r="Q867" t="n">
-        <v>137.4840000000003</v>
+        <v>137.5113333333336</v>
       </c>
       <c r="R867" t="n">
-        <v>130.47</v>
+        <v>131.29</v>
       </c>
       <c r="S867" t="n">
-        <v>130.998124112715</v>
+        <v>131.5447907793817</v>
       </c>
       <c r="T867" t="n">
-        <v>130.312407811037</v>
+        <v>130.4385616571909</v>
       </c>
       <c r="U867" t="n">
-        <v>135.9663888796604</v>
+        <v>136.0271296204012</v>
       </c>
       <c r="V867" t="n">
-        <v>-5.653981068623381</v>
+        <v>-5.588567963210295</v>
       </c>
       <c r="W867" t="n">
-        <v>-6.947001721740639</v>
+        <v>-6.933919100658022</v>
       </c>
       <c r="X867" t="n">
-        <v>1.293020653117258</v>
+        <v>1.345351137447727</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   EMA.txt 	modified:   binance_ETHUSDT_data.csv 	modified:   binance_ETHUSDT_data.xlsx 	modified:   log 	modified:   log_notify 	modified:   trade_details.csv 	modified:   trades_df.csv
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -79984,12 +79984,12 @@
       </c>
       <c r="E867" t="inlineStr">
         <is>
-          <t>131.29000000</t>
+          <t>132.03000000</t>
         </is>
       </c>
       <c r="F867" t="inlineStr">
         <is>
-          <t>267805.58315000</t>
+          <t>314337.97485000</t>
         </is>
       </c>
       <c r="G867" t="n">
@@ -79997,20 +79997,20 @@
       </c>
       <c r="H867" t="inlineStr">
         <is>
-          <t>35717036.53360180</t>
+          <t>41845455.90290630</t>
         </is>
       </c>
       <c r="I867" t="n">
-        <v>80990</v>
+        <v>99114</v>
       </c>
       <c r="J867" t="inlineStr">
         <is>
-          <t>128942.90379000</t>
+          <t>150902.67991000</t>
         </is>
       </c>
       <c r="K867" t="inlineStr">
         <is>
-          <t>17205475.24753970</t>
+          <t>20097687.06938920</t>
         </is>
       </c>
       <c r="L867" t="inlineStr">
@@ -80019,40 +80019,40 @@
         </is>
       </c>
       <c r="M867" t="n">
-        <v>131.2899999999992</v>
+        <v>132.0299999999992</v>
       </c>
       <c r="N867" t="n">
-        <v>132.8250000000002</v>
+        <v>133.1950000000002</v>
       </c>
       <c r="O867" t="n">
-        <v>128.352857142856</v>
+        <v>128.4585714285703</v>
       </c>
       <c r="P867" t="n">
-        <v>128.6020000000003</v>
+        <v>128.6513333333337</v>
       </c>
       <c r="Q867" t="n">
-        <v>137.5113333333336</v>
+        <v>137.5360000000002</v>
       </c>
       <c r="R867" t="n">
-        <v>131.29</v>
+        <v>132.03</v>
       </c>
       <c r="S867" t="n">
-        <v>131.5447907793817</v>
+        <v>132.038124112715</v>
       </c>
       <c r="T867" t="n">
-        <v>130.4385616571909</v>
+        <v>130.552407811037</v>
       </c>
       <c r="U867" t="n">
-        <v>136.0271296204012</v>
+        <v>136.081944435216</v>
       </c>
       <c r="V867" t="n">
-        <v>-5.588567963210295</v>
+        <v>-5.529536624178945</v>
       </c>
       <c r="W867" t="n">
-        <v>-6.933919100658022</v>
+        <v>-6.922112832851752</v>
       </c>
       <c r="X867" t="n">
-        <v>1.345351137447727</v>
+        <v>1.392576208672807</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   EMA.txt 	modified:   binance_ETHUSDT_data.csv 	modified:   binance_ETHUSDT_data.xlsx 	modified:   buy_sell.txt 	modified:   data.txt 	modified:   log 	modified:   log_notify 	modified:   trade_details.csv 	modified:   trades_df.csv
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_data.xlsx
+++ b/binance_ETHUSDT_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X867"/>
+  <dimension ref="A1:X872"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -79984,12 +79984,12 @@
       </c>
       <c r="E867" t="inlineStr">
         <is>
-          <t>132.03000000</t>
+          <t>131.59000000</t>
         </is>
       </c>
       <c r="F867" t="inlineStr">
         <is>
-          <t>314337.97485000</t>
+          <t>320347.21956000</t>
         </is>
       </c>
       <c r="G867" t="n">
@@ -79997,20 +79997,20 @@
       </c>
       <c r="H867" t="inlineStr">
         <is>
-          <t>41845455.90290630</t>
+          <t>42636559.38241520</t>
         </is>
       </c>
       <c r="I867" t="n">
-        <v>99114</v>
+        <v>101293</v>
       </c>
       <c r="J867" t="inlineStr">
         <is>
-          <t>150902.67991000</t>
+          <t>153829.18058000</t>
         </is>
       </c>
       <c r="K867" t="inlineStr">
         <is>
-          <t>20097687.06938920</t>
+          <t>20482964.26516290</t>
         </is>
       </c>
       <c r="L867" t="inlineStr">
@@ -80019,40 +80019,500 @@
         </is>
       </c>
       <c r="M867" t="n">
-        <v>132.0299999999992</v>
+        <v>131.5899999999992</v>
       </c>
       <c r="N867" t="n">
-        <v>133.1950000000002</v>
+        <v>132.9750000000003</v>
       </c>
       <c r="O867" t="n">
-        <v>128.4585714285703</v>
+        <v>128.3957142857132</v>
       </c>
       <c r="P867" t="n">
-        <v>128.6513333333337</v>
+        <v>128.6220000000004</v>
       </c>
       <c r="Q867" t="n">
-        <v>137.5360000000002</v>
+        <v>137.5213333333336</v>
       </c>
       <c r="R867" t="n">
-        <v>132.03</v>
+        <v>131.59</v>
       </c>
       <c r="S867" t="n">
-        <v>132.038124112715</v>
+        <v>131.7447907793817</v>
       </c>
       <c r="T867" t="n">
-        <v>130.552407811037</v>
+        <v>130.4847155033447</v>
       </c>
       <c r="U867" t="n">
-        <v>136.081944435216</v>
+        <v>136.0493518426234</v>
       </c>
       <c r="V867" t="n">
-        <v>-5.529536624178945</v>
+        <v>-5.564636339278678</v>
       </c>
       <c r="W867" t="n">
-        <v>-6.922112832851752</v>
+        <v>-6.929132775871699</v>
       </c>
       <c r="X867" t="n">
-        <v>1.392576208672807</v>
+        <v>1.36449643659302</v>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" s="1" t="n">
+        <v>866</v>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>131.61000000</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>133.68000000</t>
+        </is>
+      </c>
+      <c r="D868" t="inlineStr">
+        <is>
+          <t>128.17000000</t>
+        </is>
+      </c>
+      <c r="E868" t="inlineStr">
+        <is>
+          <t>129.16000000</t>
+        </is>
+      </c>
+      <c r="F868" t="inlineStr">
+        <is>
+          <t>264933.98418000</t>
+        </is>
+      </c>
+      <c r="G868" t="n">
+        <v>1577836799999</v>
+      </c>
+      <c r="H868" t="inlineStr">
+        <is>
+          <t>34678632.17959370</t>
+        </is>
+      </c>
+      <c r="I868" t="n">
+        <v>95085</v>
+      </c>
+      <c r="J868" t="inlineStr">
+        <is>
+          <t>131010.02709000</t>
+        </is>
+      </c>
+      <c r="K868" t="inlineStr">
+        <is>
+          <t>17146486.49368810</t>
+        </is>
+      </c>
+      <c r="L868" t="inlineStr">
+        <is>
+          <t>2019-12-31 08:00:00</t>
+        </is>
+      </c>
+      <c r="M868" t="n">
+        <v>129.1599999999992</v>
+      </c>
+      <c r="N868" t="n">
+        <v>130.3750000000002</v>
+      </c>
+      <c r="O868" t="n">
+        <v>128.5971428571417</v>
+      </c>
+      <c r="P868" t="n">
+        <v>128.3840000000004</v>
+      </c>
+      <c r="Q868" t="n">
+        <v>136.8023333333336</v>
+      </c>
+      <c r="R868" t="n">
+        <v>129.16</v>
+      </c>
+      <c r="S868" t="n">
+        <v>130.0215969264605</v>
+      </c>
+      <c r="T868" t="n">
+        <v>130.2809131182148</v>
+      </c>
+      <c r="U868" t="n">
+        <v>135.5390294839106</v>
+      </c>
+      <c r="V868" t="n">
+        <v>-5.258116365695798</v>
+      </c>
+      <c r="W868" t="n">
+        <v>-6.59492949383652</v>
+      </c>
+      <c r="X868" t="n">
+        <v>1.336813128140721</v>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" s="1" t="n">
+        <v>867</v>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>129.16000000</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>133.05000000</t>
+        </is>
+      </c>
+      <c r="D869" t="inlineStr">
+        <is>
+          <t>128.68000000</t>
+        </is>
+      </c>
+      <c r="E869" t="inlineStr">
+        <is>
+          <t>130.77000000</t>
+        </is>
+      </c>
+      <c r="F869" t="inlineStr">
+        <is>
+          <t>144770.52197000</t>
+        </is>
+      </c>
+      <c r="G869" t="n">
+        <v>1577923199999</v>
+      </c>
+      <c r="H869" t="inlineStr">
+        <is>
+          <t>18952318.53206430</t>
+        </is>
+      </c>
+      <c r="I869" t="n">
+        <v>75888</v>
+      </c>
+      <c r="J869" t="inlineStr">
+        <is>
+          <t>71847.93883000</t>
+        </is>
+      </c>
+      <c r="K869" t="inlineStr">
+        <is>
+          <t>9407940.16106830</t>
+        </is>
+      </c>
+      <c r="L869" t="inlineStr">
+        <is>
+          <t>2020-01-01 08:00:00</t>
+        </is>
+      </c>
+      <c r="M869" t="n">
+        <v>130.7699999999992</v>
+      </c>
+      <c r="N869" t="n">
+        <v>129.9650000000002</v>
+      </c>
+      <c r="O869" t="n">
+        <v>129.4085714285703</v>
+      </c>
+      <c r="P869" t="n">
+        <v>128.976666666667</v>
+      </c>
+      <c r="Q869" t="n">
+        <v>136.2063333333336</v>
+      </c>
+      <c r="R869" t="n">
+        <v>130.77</v>
+      </c>
+      <c r="S869" t="n">
+        <v>130.5205323088202</v>
+      </c>
+      <c r="T869" t="n">
+        <v>130.356157253874</v>
+      </c>
+      <c r="U869" t="n">
+        <v>135.1857680406579</v>
+      </c>
+      <c r="V869" t="n">
+        <v>-4.829610786783888</v>
+      </c>
+      <c r="W869" t="n">
+        <v>-6.241865752425994</v>
+      </c>
+      <c r="X869" t="n">
+        <v>1.412254965642106</v>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" s="1" t="n">
+        <v>868</v>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>130.72000000</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>130.78000000</t>
+        </is>
+      </c>
+      <c r="D870" t="inlineStr">
+        <is>
+          <t>126.38000000</t>
+        </is>
+      </c>
+      <c r="E870" t="inlineStr">
+        <is>
+          <t>127.19000000</t>
+        </is>
+      </c>
+      <c r="F870" t="inlineStr">
+        <is>
+          <t>213757.05806000</t>
+        </is>
+      </c>
+      <c r="G870" t="n">
+        <v>1578009599999</v>
+      </c>
+      <c r="H870" t="inlineStr">
+        <is>
+          <t>27486853.39482150</t>
+        </is>
+      </c>
+      <c r="I870" t="n">
+        <v>96193</v>
+      </c>
+      <c r="J870" t="inlineStr">
+        <is>
+          <t>105830.56192000</t>
+        </is>
+      </c>
+      <c r="K870" t="inlineStr">
+        <is>
+          <t>13615064.56872850</t>
+        </is>
+      </c>
+      <c r="L870" t="inlineStr">
+        <is>
+          <t>2020-01-02 08:00:00</t>
+        </is>
+      </c>
+      <c r="M870" t="n">
+        <v>127.1899999999992</v>
+      </c>
+      <c r="N870" t="n">
+        <v>128.9800000000002</v>
+      </c>
+      <c r="O870" t="n">
+        <v>129.6385714285703</v>
+      </c>
+      <c r="P870" t="n">
+        <v>128.6040000000004</v>
+      </c>
+      <c r="Q870" t="n">
+        <v>135.5403333333336</v>
+      </c>
+      <c r="R870" t="n">
+        <v>127.19</v>
+      </c>
+      <c r="S870" t="n">
+        <v>128.3001774362734</v>
+      </c>
+      <c r="T870" t="n">
+        <v>129.8690561378934</v>
+      </c>
+      <c r="U870" t="n">
+        <v>134.5934889265351</v>
+      </c>
+      <c r="V870" t="n">
+        <v>-4.724432788641678</v>
+      </c>
+      <c r="W870" t="n">
+        <v>-5.938379159669132</v>
+      </c>
+      <c r="X870" t="n">
+        <v>1.213946371027453</v>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" s="1" t="n">
+        <v>869</v>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>127.19000000</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>135.14000000</t>
+        </is>
+      </c>
+      <c r="D871" t="inlineStr">
+        <is>
+          <t>125.88000000</t>
+        </is>
+      </c>
+      <c r="E871" t="inlineStr">
+        <is>
+          <t>134.35000000</t>
+        </is>
+      </c>
+      <c r="F871" t="inlineStr">
+        <is>
+          <t>413055.18895000</t>
+        </is>
+      </c>
+      <c r="G871" t="n">
+        <v>1578095999999</v>
+      </c>
+      <c r="H871" t="inlineStr">
+        <is>
+          <t>54139288.21657680</t>
+        </is>
+      </c>
+      <c r="I871" t="n">
+        <v>162310</v>
+      </c>
+      <c r="J871" t="inlineStr">
+        <is>
+          <t>227899.25531000</t>
+        </is>
+      </c>
+      <c r="K871" t="inlineStr">
+        <is>
+          <t>29863547.62120130</t>
+        </is>
+      </c>
+      <c r="L871" t="inlineStr">
+        <is>
+          <t>2020-01-03 08:00:00</t>
+        </is>
+      </c>
+      <c r="M871" t="n">
+        <v>134.3499999999992</v>
+      </c>
+      <c r="N871" t="n">
+        <v>130.7700000000002</v>
+      </c>
+      <c r="O871" t="n">
+        <v>130.7899999999989</v>
+      </c>
+      <c r="P871" t="n">
+        <v>129.020666666667</v>
+      </c>
+      <c r="Q871" t="n">
+        <v>135.1726666666669</v>
+      </c>
+      <c r="R871" t="n">
+        <v>134.35</v>
+      </c>
+      <c r="S871" t="n">
+        <v>132.3333924787578</v>
+      </c>
+      <c r="T871" t="n">
+        <v>130.5584321166791</v>
+      </c>
+      <c r="U871" t="n">
+        <v>134.5754527097547</v>
+      </c>
+      <c r="V871" t="n">
+        <v>-4.017020593075642</v>
+      </c>
+      <c r="W871" t="n">
+        <v>-5.554107446350434</v>
+      </c>
+      <c r="X871" t="n">
+        <v>1.537086853274792</v>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" s="1" t="n">
+        <v>870</v>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>134.37000000</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>134.81000000</t>
+        </is>
+      </c>
+      <c r="D872" t="inlineStr">
+        <is>
+          <t>132.79000000</t>
+        </is>
+      </c>
+      <c r="E872" t="inlineStr">
+        <is>
+          <t>133.81000000</t>
+        </is>
+      </c>
+      <c r="F872" t="inlineStr">
+        <is>
+          <t>54225.72281000</t>
+        </is>
+      </c>
+      <c r="G872" t="n">
+        <v>1578182399999</v>
+      </c>
+      <c r="H872" t="inlineStr">
+        <is>
+          <t>7245234.05055340</t>
+        </is>
+      </c>
+      <c r="I872" t="n">
+        <v>27879</v>
+      </c>
+      <c r="J872" t="inlineStr">
+        <is>
+          <t>25281.39425000</t>
+        </is>
+      </c>
+      <c r="K872" t="inlineStr">
+        <is>
+          <t>3378073.84193540</t>
+        </is>
+      </c>
+      <c r="L872" t="inlineStr">
+        <is>
+          <t>2020-01-04 08:00:00</t>
+        </is>
+      </c>
+      <c r="M872" t="n">
+        <v>133.8099999999992</v>
+      </c>
+      <c r="N872" t="n">
+        <v>134.0800000000002</v>
+      </c>
+      <c r="O872" t="n">
+        <v>131.6042857142846</v>
+      </c>
+      <c r="P872" t="n">
+        <v>129.3953333333337</v>
+      </c>
+      <c r="Q872" t="n">
+        <v>134.6963333333336</v>
+      </c>
+      <c r="R872" t="n">
+        <v>133.81</v>
+      </c>
+      <c r="S872" t="n">
+        <v>133.3177974929193</v>
+      </c>
+      <c r="T872" t="n">
+        <v>131.0586733294977</v>
+      </c>
+      <c r="U872" t="n">
+        <v>134.5187525090321</v>
+      </c>
+      <c r="V872" t="n">
+        <v>-3.460079179534461</v>
+      </c>
+      <c r="W872" t="n">
+        <v>-5.13530179298724</v>
+      </c>
+      <c r="X872" t="n">
+        <v>1.675222613452779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>